<commit_message>
order cities by population
</commit_message>
<xml_diff>
--- a/cities.xlsx
+++ b/cities.xlsx
@@ -37,37 +37,37 @@
     <t>Canada</t>
   </si>
   <si>
+    <t>Marakesh</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Albuquerque</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>Los Cabos</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Greenville</t>
+  </si>
+  <si>
+    <t>Archipelago Sea</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
     <t>Pyeongchang</t>
   </si>
   <si>
     <t>South Korea</t>
-  </si>
-  <si>
-    <t>Marakesh</t>
-  </si>
-  <si>
-    <t>Morocco</t>
-  </si>
-  <si>
-    <t>Albuquerque</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>Los Cabos</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Greenville</t>
-  </si>
-  <si>
-    <t>Archipelago Sea</t>
-  </si>
-  <si>
-    <t>Finland</t>
   </si>
   <si>
     <t>Walla Walla Valley</t>
@@ -435,38 +435,38 @@
         <v>9</v>
       </c>
       <c r="C4" s="5">
-        <v>43666.0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>1464.0</v>
+        <v>928850.0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>230.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="5">
-        <v>928850.0</v>
-      </c>
-      <c r="D5" s="5">
-        <v>230.0</v>
+        <v>558545.0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>491.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="5">
-        <v>558545.0</v>
+        <v>287671.0</v>
       </c>
       <c r="D6" s="6">
-        <v>491.0</v>
+        <v>3751.0</v>
       </c>
     </row>
     <row r="7">
@@ -474,27 +474,27 @@
         <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="5">
-        <v>287671.0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>3751.0</v>
+        <v>93137.0</v>
+      </c>
+      <c r="D7" s="5">
+        <v>68.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
       <c r="C8" s="5">
-        <v>93137.0</v>
+        <v>60000.0</v>
       </c>
       <c r="D8" s="5">
-        <v>68.0</v>
+        <v>2000.0</v>
       </c>
     </row>
     <row r="9">
@@ -505,10 +505,10 @@
         <v>18</v>
       </c>
       <c r="C9" s="5">
-        <v>60000.0</v>
-      </c>
-      <c r="D9" s="5">
-        <v>2000.0</v>
+        <v>43666.0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1464.0</v>
       </c>
     </row>
     <row r="10">
@@ -516,7 +516,7 @@
         <v>19</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C10" s="5">
         <v>32986.0</v>

</xml_diff>